<commit_message>
Final logreg results update
</commit_message>
<xml_diff>
--- a/src/LogisticRegression/results/ParallelizationResults.xlsx
+++ b/src/LogisticRegression/results/ParallelizationResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alecc\Documents\Parallel Processing\eece5645-final-project\src\LogisticRegression\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2505DEA9-29EA-4858-B1E3-E3392173FE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A149DC9-B482-4FC2-B1CC-D504F646E8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40575" yWindow="2220" windowWidth="17280" windowHeight="10500" xr2:uid="{E9651202-0658-4006-904A-5A0E03BF79A5}"/>
+    <workbookView xWindow="3804" yWindow="3804" windowWidth="17280" windowHeight="10500" xr2:uid="{E9651202-0658-4006-904A-5A0E03BF79A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -73,12 +73,136 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,6 +461,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of workers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -399,6 +578,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds for 100 iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1382,7 +1616,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,139 +1625,139 @@
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>1170.7137</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>474.01470999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>307.53841999999997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>243.74136999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>224.04760999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>25</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>224.34601000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>30</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>220.70983000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>40</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>213.57199</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>50</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>206.2397</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>60</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>204.54436000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>70</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>194.84656000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>80</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>189.48811000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>90</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>194.40720999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>100</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>195.70675</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>110</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>190.15155999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
         <v>120</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>192.47393</v>
       </c>
     </row>

</xml_diff>